<commit_message>
more cleaning and analyslysis in agate
</commit_message>
<xml_diff>
--- a/0413/0413.xlsx
+++ b/0413/0413.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-400" yWindow="0" windowWidth="25040" windowHeight="15600" tabRatio="977" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="977" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="crashes_by_year" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId16"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -771,11 +771,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122201656"/>
-        <c:axId val="-2127473000"/>
+        <c:axId val="-2115557304"/>
+        <c:axId val="-2115567512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122201656"/>
+        <c:axId val="-2115557304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +784,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127473000"/>
+        <c:crossAx val="-2115567512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -792,7 +792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127473000"/>
+        <c:axId val="-2115567512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,7 +806,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122201656"/>
+        <c:crossAx val="-2115557304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -842,7 +842,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -964,11 +963,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113293528"/>
-        <c:axId val="2113566856"/>
+        <c:axId val="2062329848"/>
+        <c:axId val="2062332856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113293528"/>
+        <c:axId val="2062329848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,7 +977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113566856"/>
+        <c:crossAx val="2062332856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -986,7 +985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113566856"/>
+        <c:axId val="2062332856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,14 +996,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113293528"/>
+        <c:crossAx val="2062329848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1034,7 +1032,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1156,11 +1153,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113477864"/>
-        <c:axId val="2113395096"/>
+        <c:axId val="2062248744"/>
+        <c:axId val="2062251752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113477864"/>
+        <c:axId val="2062248744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113395096"/>
+        <c:crossAx val="2062251752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1178,7 +1175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113395096"/>
+        <c:axId val="2062251752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,14 +1186,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113477864"/>
+        <c:crossAx val="2062248744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1226,7 +1222,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1348,11 +1343,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2053367112"/>
-        <c:axId val="2113324824"/>
+        <c:axId val="2062286936"/>
+        <c:axId val="2062289944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2053367112"/>
+        <c:axId val="2062286936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113324824"/>
+        <c:crossAx val="2062289944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113324824"/>
+        <c:axId val="2062289944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,14 +1376,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053367112"/>
+        <c:crossAx val="2062286936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1418,7 +1412,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1512,11 +1505,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121895944"/>
-        <c:axId val="-2127196168"/>
+        <c:axId val="-2115764552"/>
+        <c:axId val="-2115835080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121895944"/>
+        <c:axId val="-2115764552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127196168"/>
+        <c:crossAx val="-2115835080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1533,7 +1526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127196168"/>
+        <c:axId val="-2115835080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,14 +1537,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121895944"/>
+        <c:crossAx val="-2115764552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1581,7 +1573,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1659,7 +1650,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1812,11 +1802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129463848"/>
-        <c:axId val="2106565544"/>
+        <c:axId val="-2115664888"/>
+        <c:axId val="-2115668728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129463848"/>
+        <c:axId val="-2115664888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106565544"/>
+        <c:crossAx val="-2115668728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1833,7 +1823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106565544"/>
+        <c:axId val="-2115668728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129463848"/>
+        <c:crossAx val="-2115664888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1998,11 +1988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2117301560"/>
-        <c:axId val="-2123485400"/>
+        <c:axId val="2061567560"/>
+        <c:axId val="2061563640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2117301560"/>
+        <c:axId val="2061567560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123485400"/>
+        <c:crossAx val="2061563640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,7 +2010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123485400"/>
+        <c:axId val="2061563640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2031,7 +2021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117301560"/>
+        <c:crossAx val="2061567560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2188,11 +2178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123918328"/>
-        <c:axId val="-2124441880"/>
+        <c:axId val="-2115301848"/>
+        <c:axId val="-2115127272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123918328"/>
+        <c:axId val="-2115301848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +2192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124441880"/>
+        <c:crossAx val="-2115127272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2210,7 +2200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124441880"/>
+        <c:axId val="-2115127272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123918328"/>
+        <c:crossAx val="-2115301848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2322,11 +2312,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126083816"/>
-        <c:axId val="-2118998456"/>
+        <c:axId val="-2115130632"/>
+        <c:axId val="-2115220808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126083816"/>
+        <c:axId val="-2115130632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,7 +2325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118998456"/>
+        <c:crossAx val="-2115220808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2343,7 +2333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118998456"/>
+        <c:axId val="-2115220808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126083816"/>
+        <c:crossAx val="-2115130632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2511,11 +2501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121069176"/>
-        <c:axId val="-2121062200"/>
+        <c:axId val="-2115395672"/>
+        <c:axId val="-2115392664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121069176"/>
+        <c:axId val="-2115395672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2525,7 +2515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121062200"/>
+        <c:crossAx val="-2115392664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2533,7 +2523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121062200"/>
+        <c:axId val="-2115392664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,7 +2534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121069176"/>
+        <c:crossAx val="-2115395672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2580,6 +2570,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2701,11 +2692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102447528"/>
-        <c:axId val="2112784888"/>
+        <c:axId val="2108744072"/>
+        <c:axId val="2108747080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102447528"/>
+        <c:axId val="2108744072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2715,7 +2706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112784888"/>
+        <c:crossAx val="2108747080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2723,7 +2714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112784888"/>
+        <c:axId val="2108747080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,13 +2725,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102447528"/>
+        <c:crossAx val="2108744072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2892,11 +2884,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2112259592"/>
-        <c:axId val="2112855480"/>
+        <c:axId val="2143290648"/>
+        <c:axId val="2143293656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2112259592"/>
+        <c:axId val="2143290648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112855480"/>
+        <c:crossAx val="2143293656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112855480"/>
+        <c:axId val="2143293656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2925,7 +2917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112259592"/>
+        <c:crossAx val="2143290648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2962,7 +2954,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3084,11 +3075,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2127149736"/>
-        <c:axId val="-2121950904"/>
+        <c:axId val="2062154312"/>
+        <c:axId val="2062157320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2127149736"/>
+        <c:axId val="2062154312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3098,7 +3089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121950904"/>
+        <c:crossAx val="2062157320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3106,7 +3097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121950904"/>
+        <c:axId val="2062157320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3117,14 +3108,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127149736"/>
+        <c:crossAx val="2062154312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3846,7 +3836,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E1:F48" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -7231,10 +7221,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7333,6 +7323,12 @@
       </c>
       <c r="B12" s="1">
         <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13">
+        <f>SUM(B2:B12)</f>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -7351,7 +7347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>

</xml_diff>